<commit_message>
Intro writing GWAS section and updating the summary table
I have changed the structure of this section and the following one to make it flow better
</commit_message>
<xml_diff>
--- a/Introduction/all_GWAS_studies_summary_table.xlsx
+++ b/Introduction/all_GWAS_studies_summary_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_GWAS_table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Study</t>
   </si>
@@ -168,6 +168,42 @@
   </si>
   <si>
     <t>1q31.1, 5p13.1,PLCL2,NFKBIZ, CAMK2G</t>
+  </si>
+  <si>
+    <t>19,032/39,498</t>
+  </si>
+  <si>
+    <t>CHUK, IKBKE, FASLG,KLRK1,PTEN</t>
+  </si>
+  <si>
+    <t>Largest meta-analysis so far</t>
+  </si>
+  <si>
+    <t>Bowes et al., 2015</t>
+  </si>
+  <si>
+    <t>British, Irish and Australians</t>
+  </si>
+  <si>
+    <t>1,962/8,923</t>
+  </si>
+  <si>
+    <t>PsA</t>
+  </si>
+  <si>
+    <t>PsA specific 5q31 association</t>
+  </si>
+  <si>
+    <t>1,430/1,417</t>
+  </si>
+  <si>
+    <t>Stuart et al., 2015</t>
+  </si>
+  <si>
+    <t>Fine-mapping included and additional meta-analysis including psoriaisis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PsA versus psoriasis chr18 LOC100505817, psoriasis only RGS6</t>
   </si>
 </sst>
 </file>
@@ -226,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -239,6 +275,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,23 +556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.08984375" customWidth="1"/>
-    <col min="3" max="3" width="20.90625" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="32.81640625" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -555,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -575,7 +612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -595,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -613,7 +650,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -633,7 +670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -653,7 +690,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -673,7 +710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -693,7 +730,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -713,7 +750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -731,39 +768,63 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>